<commit_message>
Todos os scripts funcionando
</commit_message>
<xml_diff>
--- a/Documentos/ICT/Platts - Lista de Índices.xlsx
+++ b/Documentos/ICT/Platts - Lista de Índices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\csnsparq2\Sup-Informacoes\UiPath\GGMP\Atualização de Índices de Mercado\Arquivos Auxiliares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Programas\Python\Extrator de texto\Documentos\ICT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494D4B0E-F58F-4478-918D-2AD0B2C28949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC94434-4FDF-48D7-B681-6813DB863852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2505" windowWidth="21300" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,19 +258,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,10 +287,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,19 +572,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +592,7 @@
         <v>20230214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -597,7 +600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -605,7 +608,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -613,7 +616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -621,7 +624,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -629,7 +632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -637,7 +640,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -645,7 +648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -653,7 +656,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -661,7 +664,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -669,7 +672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -677,17 +680,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -695,7 +698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -703,7 +706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -711,7 +714,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -719,7 +722,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -727,7 +730,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -735,7 +738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -743,7 +746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -751,7 +754,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -759,7 +762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -767,7 +770,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -775,7 +778,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -783,7 +786,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -791,7 +794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -799,7 +802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -807,7 +810,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -815,7 +818,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -823,15 +826,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -839,7 +843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -847,7 +851,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -855,7 +859,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -863,7 +867,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -873,5 +877,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>